<commit_message>
heterogeneity model with random slope
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Timestamp</t>
   </si>
@@ -74,6 +74,54 @@
   </si>
   <si>
     <t>now I have mode hunting in place</t>
+  </si>
+  <si>
+    <t>the issue of ones trick not working in jags posted on JAGS forum</t>
+  </si>
+  <si>
+    <t>5th feb 2pm</t>
+  </si>
+  <si>
+    <t>5 feb 5pm</t>
+  </si>
+  <si>
+    <t>heterogeneity model can now find intercept easily. Constrained the sum of means to be zero</t>
+  </si>
+  <si>
+    <t>5 feb 6:30pm</t>
+  </si>
+  <si>
+    <t>step(abs(mu[1] + mu[2] + mu[3]) - 0.05) doesn’t work as a good constraint. Really small values are sampled. Probably it is a better idea to freely sample params and then later transform them so that we get what we want.</t>
+  </si>
+  <si>
+    <t>6 feb 11pm</t>
+  </si>
+  <si>
+    <t>6 feb 11:30pm</t>
+  </si>
+  <si>
+    <t>in case of disproportionate proportions, even a simple GMM is difficult to estimate. It is tough to have good starting values for means but easier to do so with proportions. I think having highly disproportionate proportions at the beginning is a good idea.</t>
+  </si>
+  <si>
+    <t>Hmm probably try different proportions and see what results you get…if less label switches then choose that one.</t>
+  </si>
+  <si>
+    <t>7 Feb noon</t>
+  </si>
+  <si>
+    <t>choice of prior parameters for eta is tough especially when some of the components are nearly empty</t>
+  </si>
+  <si>
+    <t>8 Feb noon</t>
+  </si>
+  <si>
+    <t>Model with random slope running. Slow mixing and thus many estimates are quite poor.</t>
+  </si>
+  <si>
+    <t>8 Feb 1pm</t>
+  </si>
+  <si>
+    <t>Model with random slope but effects were mean centred so that fixed effects could also be estimated. Working quite well it seems, some runs were bad otherwise all parameters are estimated well</t>
   </si>
 </sst>
 </file>
@@ -119,13 +167,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -432,23 +486,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="1" max="1" width="33" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -456,7 +511,7 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -464,7 +519,7 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -472,7 +527,7 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -480,7 +535,7 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -488,23 +543,23 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -512,7 +567,7 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -520,8 +575,72 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model with complete data DIC calculation
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Timestamp</t>
   </si>
@@ -128,6 +128,24 @@
   </si>
   <si>
     <t>Marginal model working. Speed however is more or less the same.</t>
+  </si>
+  <si>
+    <t>13 feb 11am</t>
+  </si>
+  <si>
+    <t>Marginal model bayesian heterogeneity working. Way too slow speed.</t>
+  </si>
+  <si>
+    <t>13 Feb noon</t>
+  </si>
+  <si>
+    <t>Marginal model bayesian heterogeneity has less autocorrelation. Takes less number of iterations to give the same results. Also it seems it gives more accurate results with very less label switching (which can be attributed to quick convergence)</t>
+  </si>
+  <si>
+    <t>13 Feb 4:30pm</t>
+  </si>
+  <si>
+    <t>Marginal model with unequal probabilities is working. But don't put the constraints that means should be ordered or sorted. Otherwise results are a nightmare</t>
   </si>
 </sst>
 </file>
@@ -492,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,6 +675,30 @@
         <v>37</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>